<commit_message>
Moved from xlsxwriter to openpyxl.
</commit_message>
<xml_diff>
--- a/tests/data/expected-xlsx-workbook.xlsx
+++ b/tests/data/expected-xlsx-workbook.xlsx
@@ -1,57 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="worksheet-1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="worksheet-1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,17 +46,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="bold" xfId="1" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -365,34 +346,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
+    <row r="2">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="C3" t="s">
-        <v>1</v>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
+    <row r="5">
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>B5</t>
+        </is>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="C7" t="s">
-        <v>3</v>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>